<commit_message>
ARRUMANDO ANÁLISE DOS EVENTOS
</commit_message>
<xml_diff>
--- a/OPE1/AC3/analiseDosEventos.xlsx
+++ b/OPE1/AC3/analiseDosEventos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Impacta\3 semestre\Oficina de Projeto de Empresa 1\SistemaDeLojaDeRoupas\OPE1\AC3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B10E28A-A4D6-4163-A76D-88AEFAE2B609}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD95701-2B1B-4EB5-96B4-2CD94B077210}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DC2D1A34-CC0F-498C-A3F2-11C673562E31}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="69">
   <si>
     <t>Nº</t>
   </si>
@@ -219,9 +219,6 @@
     <t>x(15)</t>
   </si>
   <si>
-    <t>x(12)</t>
-  </si>
-  <si>
     <t>x(14)</t>
   </si>
   <si>
@@ -229,6 +226,12 @@
   </si>
   <si>
     <t>x(8)</t>
+  </si>
+  <si>
+    <t>Funcionário reverte produtos solicitados</t>
+  </si>
+  <si>
+    <t>Funcionário reverte saída de produtos</t>
   </si>
 </sst>
 </file>
@@ -303,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -315,9 +318,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -345,29 +345,39 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,47 +692,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DC54051-8369-4B21-8750-5327DEBE51F0}">
-  <dimension ref="A2:J54"/>
+  <dimension ref="A2:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" style="22" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" style="16" customWidth="1"/>
     <col min="4" max="4" width="54.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.21875" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.21875" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="7" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
@@ -749,10 +759,10 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="19" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="2">
@@ -771,8 +781,8 @@
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="19"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="2">
         <v>2</v>
       </c>
@@ -789,8 +799,8 @@
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="19"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="2">
         <v>3</v>
       </c>
@@ -807,8 +817,8 @@
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="19"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="2">
         <v>4</v>
       </c>
@@ -825,7 +835,7 @@
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="19"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
@@ -845,7 +855,7 @@
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="25" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -867,7 +877,7 @@
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="18"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
@@ -882,7 +892,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J10" s="4"/>
     </row>
@@ -890,7 +900,7 @@
       <c r="A11" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="19" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="2">
@@ -910,7 +920,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="20"/>
-      <c r="B12" s="7"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="2">
         <v>9</v>
       </c>
@@ -918,7 +928,7 @@
         <v>19</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -928,7 +938,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="20"/>
-      <c r="B13" s="7"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="2">
         <v>10</v>
       </c>
@@ -946,11 +956,11 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="20"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="13">
+      <c r="B14" s="19"/>
+      <c r="C14" s="12">
         <v>11</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="13" t="s">
         <v>26</v>
       </c>
       <c r="E14" s="4"/>
@@ -964,7 +974,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="20"/>
-      <c r="B15" s="7"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="2">
         <v>12</v>
       </c>
@@ -982,7 +992,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="20"/>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="19" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="2">
@@ -1002,139 +1012,139 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="20"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="13">
+      <c r="B17" s="19"/>
+      <c r="C17" s="5">
         <v>14</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="20"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="12">
+        <v>15</v>
+      </c>
+      <c r="D18" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4" t="s">
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="7" t="s">
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7" t="s">
+      <c r="F20" s="19"/>
+      <c r="G20" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="2" t="s">
+      <c r="B21" s="21"/>
+      <c r="C21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F21" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G21" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="I21" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="J21" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="17" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B22" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C22" s="2">
         <v>1</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4" t="s">
+      <c r="E22" s="4"/>
+      <c r="F22" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="2">
-        <v>2</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
-      <c r="B23" s="7"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>55</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="G23" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
-      <c r="B24" s="7"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="19"/>
       <c r="C24" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -1143,54 +1153,54 @@
       <c r="J24" s="4"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="13">
-        <v>5</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E25" s="4"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="2">
+        <v>4</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="F25" s="4"/>
-      <c r="G25" s="4" t="s">
-        <v>57</v>
-      </c>
+      <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
-      <c r="B26" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="2">
-        <v>6</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="A26" s="18"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="12">
+        <v>5</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+      <c r="G26" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
-      <c r="B27" s="7"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="19" t="s">
+        <v>15</v>
+      </c>
       <c r="C27" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
@@ -1199,74 +1209,74 @@
       <c r="J27" s="4"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="17"/>
-      <c r="B28" s="7"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E28" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
-      <c r="I28" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="I28" s="4"/>
       <c r="J28" s="4"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>16</v>
-      </c>
+      <c r="A29" s="18"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
-      <c r="H29" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="J29" s="4"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="18"/>
-      <c r="B30" s="7"/>
+      <c r="A30" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>16</v>
+      </c>
       <c r="C30" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>60</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
+      <c r="H30" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="18"/>
-      <c r="B31" s="7"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -1275,232 +1285,232 @@
       <c r="J31" s="4"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="18"/>
-      <c r="B32" s="7"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="19"/>
       <c r="C32" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="F32" s="4"/>
-      <c r="G32" s="4" t="s">
-        <v>62</v>
-      </c>
+      <c r="G32" s="4"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="18"/>
-      <c r="B33" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="A33" s="25"/>
+      <c r="B33" s="19"/>
       <c r="C33" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>64</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E33" s="4"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
+      <c r="G33" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>16</v>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="25"/>
+      <c r="B34" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C34" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E34" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
-      <c r="H34" s="4" t="s">
-        <v>52</v>
-      </c>
+      <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="20"/>
-      <c r="B35" s="7"/>
+    <row r="35" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>16</v>
+      </c>
       <c r="C35" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>65</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
+      <c r="H35" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="20"/>
-      <c r="B36" s="7"/>
+      <c r="B36" s="19"/>
       <c r="C36" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E36" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="F36" s="4"/>
-      <c r="G36" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="20"/>
-      <c r="B37" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="B37" s="19"/>
       <c r="C37" s="2">
-        <v>17</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>53</v>
+        <v>16</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
+      <c r="G37" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
-      <c r="J37" s="4" t="s">
+      <c r="J37" s="4"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="20"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="5">
+        <v>17</v>
+      </c>
+      <c r="D38" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="20"/>
+      <c r="B39" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="2">
+        <v>18</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="21"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="15"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="7" t="s">
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7" t="s">
+      <c r="F41" s="19"/>
+      <c r="G41" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="4"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" s="6" t="s">
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="4"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="2" t="s">
+      <c r="B42" s="21"/>
+      <c r="C42" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E42" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F42" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="G42" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H40" s="4" t="s">
+      <c r="H42" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I40" s="4" t="s">
+      <c r="I42" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J40" s="4" t="s">
+      <c r="J42" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="17" t="s">
+    <row r="43" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B43" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C43" s="2">
         <v>1</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E43" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="17"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="2">
-        <v>2</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="17"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="2">
-        <v>3</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -1509,174 +1519,210 @@
       <c r="J43" s="4"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="17"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="13">
-        <v>4</v>
-      </c>
-      <c r="D44" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E44" s="4"/>
+      <c r="A44" s="18"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="2">
+        <v>2</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="F44" s="4"/>
-      <c r="G44" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="G44" s="4"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="21"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="16"/>
-      <c r="J45" s="16"/>
+      <c r="A45" s="18"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="2">
+        <v>3</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="21"/>
-      <c r="B46" s="15"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="16"/>
-      <c r="I46" s="16"/>
-      <c r="J46" s="16"/>
-    </row>
-    <row r="47" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="21"/>
-      <c r="B47" s="15"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
-      <c r="H47" s="16"/>
-      <c r="I47" s="16"/>
-      <c r="J47" s="16"/>
+      <c r="A46" s="18"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="12">
+        <v>4</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="15"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48" s="21"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="16"/>
-      <c r="G48" s="16"/>
-      <c r="H48" s="16"/>
-      <c r="I48" s="16"/>
-      <c r="J48" s="16"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" s="21"/>
-      <c r="B49" s="15"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="16"/>
-      <c r="H49" s="16"/>
-      <c r="I49" s="16"/>
-      <c r="J49" s="16"/>
+      <c r="A48" s="15"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+    </row>
+    <row r="49" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="15"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="14"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" s="21"/>
-      <c r="B50" s="15"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="16"/>
-      <c r="H50" s="16"/>
-      <c r="I50" s="16"/>
-      <c r="J50" s="16"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" s="21"/>
-      <c r="B51" s="16"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="16"/>
-      <c r="H51" s="16"/>
-      <c r="I51" s="16"/>
-      <c r="J51" s="16"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52" s="21"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="16"/>
-      <c r="H52" s="16"/>
-      <c r="I52" s="16"/>
-      <c r="J52" s="16"/>
+      <c r="A52" s="15"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A53" s="21"/>
-      <c r="B53" s="12"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="16"/>
-      <c r="G53" s="16"/>
-      <c r="H53" s="16"/>
-      <c r="I53" s="16"/>
-      <c r="J53" s="16"/>
+      <c r="A53" s="15"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A54" s="21"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="16"/>
-      <c r="H54" s="16"/>
-      <c r="I54" s="16"/>
-      <c r="J54" s="16"/>
+      <c r="A54" s="15"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" s="15"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="14"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" s="15"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A11:A17"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="A21:A28"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="A20:D20"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="A4:A8"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="A35:A39"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="A22:A29"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B22:B26"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>